<commit_message>
Mise à jour Backlog et Planning
</commit_message>
<xml_diff>
--- a/Reponse-appel-offre/Macro-planning.xlsx
+++ b/Reponse-appel-offre/Macro-planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romainpasquier/PhpstormProjects/MasterCamp/Reponse-appel-offre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE519E7-16E2-7746-97AA-C0EF647099C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038FD4F1-13C4-8748-965B-404276FC853B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20520" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Votre projet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Détails du projet</t>
   </si>
@@ -158,6 +158,30 @@
   </si>
   <si>
     <t>’</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>Implementation backend beta</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>Implementation Frontend beta</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>Réflechir aux questions de confiance et de sécurité</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>Réfléchir au déploiement de l'app</t>
   </si>
 </sst>
 </file>
@@ -444,40 +468,40 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -966,7 +990,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -983,57 +1007,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="G1" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="12" x14ac:dyDescent="0.15">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="G2" s="2">
         <f ca="1">TODAY()</f>
-        <v>44729</v>
+        <v>44731</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="12" x14ac:dyDescent="0.15">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:34" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="22"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:34" ht="12" x14ac:dyDescent="0.15">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="29" t="s">
         <v>6</v>
       </c>
@@ -1042,10 +1066,10 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:34" ht="12" x14ac:dyDescent="0.15">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="24">
         <v>44721</v>
       </c>
@@ -1054,13 +1078,13 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:34" s="3" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="14"/>
       <c r="G7" s="11"/>
       <c r="H7" s="4">
@@ -1285,19 +1309,19 @@
       </c>
     </row>
     <row r="9" spans="1:34" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="41" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="13"/>
@@ -1411,11 +1435,11 @@
       </c>
     </row>
     <row r="10" spans="1:34" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="31"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13"/>
       <c r="H10" s="8">
         <f>DAY(H7)</f>
@@ -1736,11 +1760,11 @@
         <v>44731</v>
       </c>
       <c r="F16" s="15">
-        <v>0.8</v>
+        <v>100</v>
       </c>
       <c r="G16" s="16">
         <f t="shared" si="7"/>
-        <v>44730.6</v>
+        <v>44929</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -1757,14 +1781,14 @@
         <v>10</v>
       </c>
       <c r="E17" s="28">
-        <f t="shared" si="8"/>
+        <f>IF(B17="","",IF($C$5="OUI",WORKDAY(C17,IF(WEEKDAY(C17,2)&gt;=6,D17,D17-1)),C17+D17-1))</f>
         <v>44740</v>
       </c>
       <c r="F17" s="15">
         <v>0</v>
       </c>
       <c r="G17" s="16">
-        <f t="shared" si="7"/>
+        <f>C17+F17*(E17-C17)</f>
         <v>44731</v>
       </c>
     </row>
@@ -1782,14 +1806,14 @@
         <v>10</v>
       </c>
       <c r="E18" s="28">
-        <f t="shared" si="8"/>
+        <f>IF(B18="","",IF($C$5="OUI",WORKDAY(C18,IF(WEEKDAY(C18,2)&gt;=6,D18,D18-1)),C18+D18-1))</f>
         <v>44740</v>
       </c>
       <c r="F18" s="15">
         <v>0</v>
       </c>
       <c r="G18" s="16">
-        <f t="shared" si="7"/>
+        <f>C18+F18*(E18-C18)</f>
         <v>44731</v>
       </c>
     </row>
@@ -1807,14 +1831,14 @@
         <v>4</v>
       </c>
       <c r="E19" s="28">
-        <f t="shared" si="8"/>
+        <f>IF(B19="","",IF($C$5="OUI",WORKDAY(C19,IF(WEEKDAY(C19,2)&gt;=6,D19,D19-1)),C19+D19-1))</f>
         <v>44743</v>
       </c>
       <c r="F19" s="15">
         <v>0</v>
       </c>
       <c r="G19" s="16">
-        <f t="shared" si="7"/>
+        <f>C19+F19*(E19-C19)</f>
         <v>44740</v>
       </c>
     </row>
@@ -1832,14 +1856,14 @@
         <v>4</v>
       </c>
       <c r="E20" s="28">
-        <f t="shared" si="8"/>
+        <f>IF(B20="","",IF($C$5="OUI",WORKDAY(C20,IF(WEEKDAY(C20,2)&gt;=6,D20,D20-1)),C20+D20-1))</f>
         <v>44746</v>
       </c>
       <c r="F20" s="15">
         <v>0</v>
       </c>
       <c r="G20" s="16">
-        <f t="shared" si="7"/>
+        <f>C20+F20*(E20-C20)</f>
         <v>44743</v>
       </c>
     </row>
@@ -1851,59 +1875,111 @@
         <v/>
       </c>
       <c r="G21" s="16" t="e">
+        <f>C21+F21*(E21-C21)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI21" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="30">
+        <v>44732</v>
+      </c>
+      <c r="D22" s="9">
+        <v>3</v>
+      </c>
+      <c r="E22" s="28">
+        <f t="shared" si="8"/>
+        <v>44734</v>
+      </c>
+      <c r="F22" s="15">
+        <v>0</v>
+      </c>
+      <c r="G22" s="16">
+        <f>C22+F22*(E22-C22)</f>
+        <v>44732</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="30">
+        <v>44732</v>
+      </c>
+      <c r="D23" s="9">
+        <v>3</v>
+      </c>
+      <c r="E23" s="28">
+        <f t="shared" ref="E23" si="9">IF(B23="","",IF($C$5="OUI",WORKDAY(C23,IF(WEEKDAY(C23,2)&gt;=6,D23,D23-1)),C23+D23-1))</f>
+        <v>44734</v>
+      </c>
+      <c r="F23" s="15">
+        <v>0</v>
+      </c>
+      <c r="G23" s="16">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AI21" s="42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C22" s="30"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="28" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G22" s="16" t="e">
+        <v>44732</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="30">
+        <v>44732</v>
+      </c>
+      <c r="D24" s="9">
+        <v>3</v>
+      </c>
+      <c r="E24" s="28">
+        <f t="shared" si="8"/>
+        <v>44734</v>
+      </c>
+      <c r="F24" s="15">
+        <v>0</v>
+      </c>
+      <c r="G24" s="16">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C23" s="30"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="28" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G23" s="16" t="e">
+        <v>44732</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="30">
+        <v>44732</v>
+      </c>
+      <c r="D25" s="9">
+        <v>7</v>
+      </c>
+      <c r="E25" s="28">
+        <f t="shared" si="8"/>
+        <v>44738</v>
+      </c>
+      <c r="F25" s="15">
+        <v>0</v>
+      </c>
+      <c r="G25" s="16">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C24" s="30"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="28" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G24" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="30"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="28" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G25" s="16" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+        <v>44732</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -2298,144 +2374,149 @@
     </row>
     <row r="76" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E76" s="28" t="str">
-        <f t="shared" ref="E76:E98" si="9">IF(B76="","",IF($C$5="OUI",WORKDAY(C76,IF(WEEKDAY(C76,2)&gt;=6,D76,D76-1)),C76+D76-1))</f>
+        <f t="shared" ref="E76:E98" si="10">IF(B76="","",IF($C$5="OUI",WORKDAY(C76,IF(WEEKDAY(C76,2)&gt;=6,D76,D76-1)),C76+D76-1))</f>
         <v/>
       </c>
     </row>
     <row r="77" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E77" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E78" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E79" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E80" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E81" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E82" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E83" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E84" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E85" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E86" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E87" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E88" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E89" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E90" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E91" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="5:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E92" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E93" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E94" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E95" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E96" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E97" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E98" s="28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C2:E2"/>
@@ -2445,11 +2526,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="H8:AH8">
     <cfRule type="expression" dxfId="8" priority="12">
@@ -2612,26 +2688,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b77de7d0-dd41-47ef-864a-ef89e53446d1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7d684a28-ca2c-49ae-9c17-671fbe8cbec0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F260FF8688AB5D4FA38BC59D128BAA5D" ma:contentTypeVersion="10" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e38acdcbce08faf09eb9c97b9601f6f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b77de7d0-dd41-47ef-864a-ef89e53446d1" xmlns:ns3="7d684a28-ca2c-49ae-9c17-671fbe8cbec0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="043768d237c07e1330d37e055f949481" ns2:_="" ns3:_="">
     <xsd:import namespace="b77de7d0-dd41-47ef-864a-ef89e53446d1"/>
@@ -2820,26 +2876,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AD40320-3ADC-4F6F-AC77-69E654FA80F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b77de7d0-dd41-47ef-864a-ef89e53446d1"/>
-    <ds:schemaRef ds:uri="7d684a28-ca2c-49ae-9c17-671fbe8cbec0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137FA1DB-8DA8-485D-B6B6-1AE808D7449C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b77de7d0-dd41-47ef-864a-ef89e53446d1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7d684a28-ca2c-49ae-9c17-671fbe8cbec0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BD25C60-5194-42BD-B3B7-33D7D498FF44}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2856,4 +2913,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137FA1DB-8DA8-485D-B6B6-1AE808D7449C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AD40320-3ADC-4F6F-AC77-69E654FA80F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b77de7d0-dd41-47ef-864a-ef89e53446d1"/>
+    <ds:schemaRef ds:uri="7d684a28-ca2c-49ae-9c17-671fbe8cbec0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update des id des models
</commit_message>
<xml_diff>
--- a/Reponse-appel-offre/Macro-planning.xlsx
+++ b/Reponse-appel-offre/Macro-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romainpasquier/PhpstormProjects/MasterCamp/Reponse-appel-offre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB28561-23DC-4949-9FD8-AA98EEDB924A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26A9796-B4AF-D949-8EDC-54933CCA2555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,38 +469,38 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -990,7 +990,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -1007,57 +1007,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="G1" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="12" x14ac:dyDescent="0.15">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="G2" s="2">
         <f ca="1">TODAY()</f>
-        <v>44731</v>
+        <v>44732</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="12" x14ac:dyDescent="0.15">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="37" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:34" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="22"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:34" ht="12" x14ac:dyDescent="0.15">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="29" t="s">
         <v>6</v>
       </c>
@@ -1066,10 +1066,10 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:34" ht="12" x14ac:dyDescent="0.15">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="40"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="24">
         <v>44721</v>
       </c>
@@ -1078,13 +1078,13 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:34" s="3" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="14"/>
       <c r="G7" s="11"/>
       <c r="H7" s="4">
@@ -1309,19 +1309,19 @@
       </c>
     </row>
     <row r="9" spans="1:34" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="41" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="13"/>
@@ -1435,11 +1435,11 @@
       </c>
     </row>
     <row r="10" spans="1:34" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="32"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13"/>
       <c r="H10" s="8">
         <f>DAY(H7)</f>
@@ -1785,11 +1785,11 @@
         <v>44740</v>
       </c>
       <c r="F17" s="15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G17" s="16">
         <f t="shared" ref="G17:G22" si="9">C17+F17*(E17-C17)</f>
-        <v>44731</v>
+        <v>44731.9</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -1810,11 +1810,11 @@
         <v>44740</v>
       </c>
       <c r="F18" s="15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G18" s="16">
         <f t="shared" si="9"/>
-        <v>44731</v>
+        <v>44731.9</v>
       </c>
     </row>
     <row r="19" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -1893,18 +1893,18 @@
         <v>44732</v>
       </c>
       <c r="D22" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" s="28">
         <f t="shared" si="8"/>
-        <v>44734</v>
+        <v>44735</v>
       </c>
       <c r="F22" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G22" s="16">
         <f t="shared" si="9"/>
-        <v>44732</v>
+        <v>44732.6</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -1918,18 +1918,18 @@
         <v>44732</v>
       </c>
       <c r="D23" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" ref="E23" si="10">IF(B23="","",IF($C$5="OUI",WORKDAY(C23,IF(WEEKDAY(C23,2)&gt;=6,D23,D23-1)),C23+D23-1))</f>
-        <v>44734</v>
+        <v>44735</v>
       </c>
       <c r="F23" s="15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G23" s="16">
         <f t="shared" si="7"/>
-        <v>44732</v>
+        <v>44732.3</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -2512,6 +2512,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C2:E2"/>
@@ -2521,11 +2526,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="H8:AH8">
     <cfRule type="expression" dxfId="8" priority="12">
@@ -2688,12 +2688,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b77de7d0-dd41-47ef-864a-ef89e53446d1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7d684a28-ca2c-49ae-9c17-671fbe8cbec0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2886,20 +2888,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b77de7d0-dd41-47ef-864a-ef89e53446d1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7d684a28-ca2c-49ae-9c17-671fbe8cbec0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137FA1DB-8DA8-485D-B6B6-1AE808D7449C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AD40320-3ADC-4F6F-AC77-69E654FA80F1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b77de7d0-dd41-47ef-864a-ef89e53446d1"/>
+    <ds:schemaRef ds:uri="7d684a28-ca2c-49ae-9c17-671fbe8cbec0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2924,12 +2927,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AD40320-3ADC-4F6F-AC77-69E654FA80F1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137FA1DB-8DA8-485D-B6B6-1AE808D7449C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b77de7d0-dd41-47ef-864a-ef89e53446d1"/>
-    <ds:schemaRef ds:uri="7d684a28-ca2c-49ae-9c17-671fbe8cbec0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>